<commit_message>
fixed a few issues
</commit_message>
<xml_diff>
--- a/ac translations/Greek.xlsx
+++ b/ac translations/Greek.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\Remote - Projects\helper projects\Remotes App Translation Project\ac translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvi\Desktop\dev\helpers\translation fetcher\ac translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="English Translation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1229,6 +1229,9 @@
 TV remote control for your click play set top case</t>
   </si>
   <si>
+    <t>App Description</t>
+  </si>
+  <si>
     <t>ΔΩΡΕΑΝ έκδοση για περιορισμένο χρονικό διάστημα
 Χάσατε το τηλεχειριστήριο του κλιματιστικού σας; κανένα πρόβλημα!
 **ΑΠΟΠΟΙΗΣΗ ΕΥΘΥΝΩΝ
@@ -1239,8 +1242,6 @@
 Δεν είστε σίγουροι τι σημαίνει αυτό; μπορείτε να δοκιμάσετε να κάνετε λήψη της εφαρμογής και να δείτε εάν λειτουργεί
 Το τηλεχειριστήριο σας λείπει; Απλά ζητήστε το από εμάς από την εφαρμογή
 Χαρακτηριστικά:
-* Ελέγξτε την τηλεόρασή ____ σας από το τηλέφωνό σας
-* Ελέγξτε την ΕΝΤΑΣΗ ΗΧΟΥ της τηλεόρασή σας (πάνω/κάτω/σίγαση/ήχος βίντεο)
 * ΑΠΟΘΗΚΕΥΣΤΕ τα αγαπημένα σας τηλεχειριστήρια για εύκολη πρόσβαση
 * ΧΩΡΙΣ εγκατάσταση, απλά κάντε κλικ και πατήστε
 * Εκπληκτικός σχεδιασμός με δροσερή και εύκολη διεπαφή
@@ -1248,14 +1249,11 @@
 Μη διστάσετε να επικοινωνήσετε μαζί μας στην _____
 Τηλεχειριστήριο τηλεόρασης για την κλικ παιχνίδι τοποθέτηση κορυφαία θήκη</t>
   </si>
-  <si>
-    <t>App Description</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -1733,11 +1731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3365,7 +3363,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="12.75" customHeight="1">
+    <row r="136" spans="1:6" ht="292.5" customHeight="1">
       <c r="A136" s="14" t="s">
         <v>395</v>
       </c>
@@ -3373,10 +3371,10 @@
         <v>396</v>
       </c>
       <c r="C136" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="F136" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>